<commit_message>
add deepseek to Elevate
</commit_message>
<xml_diff>
--- a/dataset_2022/benchmark_stable.xlsx
+++ b/dataset_2022/benchmark_stable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IoT\4-Elevate\GPT4_vitas\dataset_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C780E8-C27A-4F9E-9189-F1B828953D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464351B8-742A-41CF-917D-B6A03BE98B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="960" windowWidth="13280" windowHeight="11220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -2645,7 +2645,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2654,13 +2654,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2693,7 +2687,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2702,18 +2696,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3031,8 +3028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3113,287 +3110,287 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>536</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="L2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>1.9</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="7">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="O3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="L4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" s="2" t="s">
+      <c r="O4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="L5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3468,926 +3465,926 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="L7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W7" t="s">
+      <c r="W7" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="7">
         <v>5</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L8" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="L8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:23" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>3.4</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>9</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="F9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="4" t="s">
+      <c r="L9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="N9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="4" t="s">
+      <c r="N9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="S9" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="T9" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="U9" s="4" t="s">
+      <c r="U9" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="V9" s="4" t="s">
+      <c r="V9" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="W9" s="4" t="s">
+      <c r="W9" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="7">
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="7">
         <v>89</v>
       </c>
-      <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="F10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S10" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="V10" t="s">
+      <c r="V10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W10" t="s">
+      <c r="W10" s="7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:23" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="L11" t="s">
-        <v>1</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="L11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="N11" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="2" t="s">
+      <c r="N11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S11" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="V11" t="s">
+      <c r="V11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4" t="s">
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="4" t="s">
+      <c r="L12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="N12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="5" t="s">
+      <c r="N12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="S12" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="T12" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="U12" s="4" t="s">
+      <c r="U12" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="V12" s="4" t="s">
+      <c r="V12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W12" s="4" t="s">
+      <c r="W12" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="7">
         <v>2</v>
       </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" s="4" t="s">
+      <c r="L13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P13" s="4" t="s">
+      <c r="N13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="Q13" s="4" t="s">
+      <c r="Q13" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="S13" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="T13" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="U13" s="4" t="s">
+      <c r="U13" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="V13" s="4" t="s">
+      <c r="V13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W13" s="4" t="s">
+      <c r="W13" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:23" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L14" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="L14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="N14" t="s">
-        <v>3</v>
-      </c>
-      <c r="O14" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="2" t="s">
+      <c r="N14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U14" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="V14" t="s">
+      <c r="V14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W14" t="s">
+      <c r="W14" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:23" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="5">
         <v>5</v>
       </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="4" t="s">
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M15" s="4" t="s">
+      <c r="L15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="N15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P15" s="5" t="s">
+      <c r="N15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="Q15" s="4" t="s">
+      <c r="Q15" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="S15" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="T15" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="U15" s="4" t="s">
+      <c r="U15" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="V15" s="4" t="s">
+      <c r="V15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W15" s="4" t="s">
+      <c r="W15" s="5" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:23" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <v>5</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
+      <c r="L16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="O16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P16" t="s">
+      <c r="O16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P16" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S16" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T16" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="U16" t="s">
+      <c r="U16" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="V16" t="s">
+      <c r="V16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W16" t="s">
+      <c r="W16" s="5" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="1:23" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:23" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>5</v>
       </c>
-      <c r="E17" s="6">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="K17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" s="6" t="s">
+      <c r="L17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="N17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O17" s="6" t="s">
+      <c r="N17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P17" s="6" t="s">
+      <c r="P17" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="Q17" s="6" t="s">
+      <c r="Q17" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="R17" s="6" t="s">
+      <c r="R17" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="S17" s="6" t="s">
+      <c r="S17" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="T17" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="U17" s="6" t="s">
+      <c r="U17" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="V17" s="6" t="s">
+      <c r="V17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W17" s="6" t="s">
+      <c r="W17" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:23" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="D18" s="6">
-        <v>0</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L18" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" s="6" t="s">
+      <c r="L18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="N18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P18" s="7" t="s">
+      <c r="N18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="Q18" s="6" t="s">
+      <c r="Q18" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="R18" s="6" t="s">
+      <c r="R18" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="S18" s="6" t="s">
+      <c r="S18" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="T18" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="U18" s="6" t="s">
+      <c r="U18" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="V18" s="6" t="s">
+      <c r="V18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W18" s="6" t="s">
+      <c r="W18" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:23" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="5">
         <v>2.6</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="5">
         <v>2</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="4" t="s">
+      <c r="F19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="L19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" s="4" t="s">
+      <c r="L19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="N19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P19" s="5" t="s">
+      <c r="N19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="Q19" s="4" t="s">
+      <c r="Q19" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="S19" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="T19" s="4" t="s">
+      <c r="T19" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="U19" s="4" t="s">
+      <c r="U19" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="V19" s="4" t="s">
+      <c r="V19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W19" s="4" t="s">
+      <c r="W19" s="5" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5441,538 +5438,538 @@
         <v>504</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>505</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="D35" s="7">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="G35" t="s">
-        <v>1</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="G35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="7" t="s">
         <v>508</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K35" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L35" t="s">
-        <v>1</v>
-      </c>
-      <c r="M35" t="s">
+      <c r="L35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" s="7" t="s">
         <v>510</v>
       </c>
-      <c r="N35" t="s">
-        <v>3</v>
-      </c>
-      <c r="O35" t="s">
-        <v>3</v>
-      </c>
-      <c r="P35" t="s">
+      <c r="N35" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O35" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P35" s="7" t="s">
         <v>511</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="Q35" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="U35" t="s">
+      <c r="U35" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="V35" t="s">
+      <c r="V35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W35" t="s">
+      <c r="W35" s="7" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="7" t="s">
         <v>514</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="7">
         <v>2.5</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="7">
         <v>1630</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="G36" t="s">
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="G36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" s="7" t="s">
         <v>516</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="7" t="s">
         <v>517</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L36" t="s">
-        <v>1</v>
-      </c>
-      <c r="M36" t="s">
+      <c r="L36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M36" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="N36" t="s">
-        <v>3</v>
-      </c>
-      <c r="O36" t="s">
-        <v>3</v>
-      </c>
-      <c r="P36" t="s">
+      <c r="N36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P36" s="7" t="s">
         <v>519</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="Q36" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="U36" t="s">
+      <c r="U36" s="7" t="s">
         <v>520</v>
       </c>
-      <c r="V36" t="s">
+      <c r="V36" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W36" t="s">
+      <c r="W36" s="7" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>521</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="7">
         <v>4</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="7">
         <v>5</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="G37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="G37" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L37" t="s">
-        <v>1</v>
-      </c>
-      <c r="M37" t="s">
+      <c r="L37" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M37" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="N37" t="s">
-        <v>3</v>
-      </c>
-      <c r="O37" t="s">
-        <v>3</v>
-      </c>
-      <c r="P37" t="s">
+      <c r="N37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P37" s="7" t="s">
         <v>527</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="Q37" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="U37" t="s">
+      <c r="U37" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="V37" t="s">
+      <c r="V37" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W37" t="s">
+      <c r="W37" s="7" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38" t="s">
-        <v>0</v>
-      </c>
-      <c r="G38" t="s">
-        <v>1</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="D38" s="7">
+        <v>0</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="L38" t="s">
-        <v>1</v>
-      </c>
-      <c r="M38" t="s">
+      <c r="L38" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M38" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="N38" t="s">
-        <v>3</v>
-      </c>
-      <c r="O38" t="s">
-        <v>3</v>
-      </c>
-      <c r="P38" t="s">
+      <c r="N38" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P38" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="Q38" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="R38" t="s">
+      <c r="R38" s="7" t="s">
         <v>462</v>
       </c>
-      <c r="S38" t="s">
+      <c r="S38" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="T38" t="s">
+      <c r="T38" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="U38" t="s">
+      <c r="U38" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="V38" t="s">
+      <c r="V38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W38" t="s">
+      <c r="W38" s="7" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="7">
         <v>5</v>
       </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>0</v>
-      </c>
-      <c r="G39" t="s">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
+      <c r="E39" s="7">
+        <v>1</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K39" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="L39" t="s">
-        <v>1</v>
-      </c>
-      <c r="M39" t="s">
+      <c r="L39" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M39" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="N39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O39" t="s">
-        <v>3</v>
-      </c>
-      <c r="P39" t="s">
+      <c r="N39" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P39" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="Q39" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="R39" t="s">
+      <c r="R39" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="S39" t="s">
+      <c r="S39" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="T39" t="s">
+      <c r="T39" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="U39" t="s">
+      <c r="U39" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="V39" t="s">
+      <c r="V39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W39" t="s">
+      <c r="W39" s="7" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:26" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="7">
         <v>3.4</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="7">
         <v>1035</v>
       </c>
-      <c r="F40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G40" t="s">
-        <v>1</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="F40" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="7" t="s">
         <v>529</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="L40" t="s">
-        <v>1</v>
-      </c>
-      <c r="M40" t="s">
+      <c r="L40" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M40" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="N40" t="s">
-        <v>3</v>
-      </c>
-      <c r="O40" t="s">
-        <v>3</v>
-      </c>
-      <c r="P40" s="8" t="s">
+      <c r="N40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P40" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="Q40" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="R40" t="s">
+      <c r="R40" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="S40" t="s">
+      <c r="S40" s="7" t="s">
         <v>488</v>
       </c>
-      <c r="T40" t="s">
+      <c r="T40" s="7" t="s">
         <v>489</v>
       </c>
-      <c r="U40" t="s">
+      <c r="U40" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="V40" t="s">
+      <c r="V40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W40" t="s">
+      <c r="W40" s="7" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>531</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="7">
         <v>4</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="7">
         <v>823</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="G41" t="s">
-        <v>1</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="G41" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="7" t="s">
         <v>532</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="L41" t="s">
-        <v>1</v>
-      </c>
-      <c r="M41" t="s">
+      <c r="L41" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M41" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="N41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O41" t="s">
-        <v>3</v>
-      </c>
-      <c r="P41" t="s">
+      <c r="N41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P41" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="Q41" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="U41" t="s">
+      <c r="U41" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="V41" t="s">
+      <c r="V41" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W41" t="s">
+      <c r="W41" s="7" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:26" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="7" t="s">
         <v>596</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="7" t="s">
         <v>539</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42" t="s">
-        <v>0</v>
-      </c>
-      <c r="G42" t="s">
-        <v>1</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="D42" s="7">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="L42" t="s">
-        <v>1</v>
-      </c>
-      <c r="M42" t="s">
+      <c r="L42" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M42" s="7" t="s">
         <v>542</v>
       </c>
-      <c r="N42" t="s">
-        <v>3</v>
-      </c>
-      <c r="O42" t="s">
-        <v>3</v>
-      </c>
-      <c r="P42" t="s">
+      <c r="N42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P42" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="Q42" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="R42" t="s">
+      <c r="R42" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="S42" t="s">
+      <c r="S42" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="T42" t="s">
+      <c r="T42" s="7" t="s">
         <v>546</v>
       </c>
-      <c r="U42" t="s">
+      <c r="U42" s="7" t="s">
         <v>547</v>
       </c>
-      <c r="V42" t="s">
+      <c r="V42" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W42" t="s">
+      <c r="W42" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="Z42" t="s">
+      <c r="Z42" s="7" t="s">
         <v>549</v>
       </c>
     </row>
@@ -6022,7 +6019,7 @@
       <c r="O43" t="s">
         <v>4</v>
       </c>
-      <c r="P43" s="8" t="s">
+      <c r="P43" s="4" t="s">
         <v>557</v>
       </c>
       <c r="Q43" t="s">
@@ -6050,77 +6047,77 @@
         <v>564</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:26" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>565</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="7" t="s">
         <v>681</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="7" t="s">
         <v>566</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44" t="s">
-        <v>0</v>
-      </c>
-      <c r="G44" t="s">
-        <v>1</v>
-      </c>
-      <c r="H44" t="s">
+      <c r="D44" s="7">
+        <v>0</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="7" t="s">
         <v>568</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K44" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L44" t="s">
-        <v>1</v>
-      </c>
-      <c r="M44" t="s">
+      <c r="L44" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M44" s="7" t="s">
         <v>570</v>
       </c>
-      <c r="N44" t="s">
-        <v>3</v>
-      </c>
-      <c r="O44" t="s">
-        <v>3</v>
-      </c>
-      <c r="P44" s="8" t="s">
+      <c r="N44" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P44" s="9" t="s">
         <v>571</v>
       </c>
-      <c r="Q44" t="s">
+      <c r="Q44" s="7" t="s">
         <v>572</v>
       </c>
-      <c r="R44" t="s">
+      <c r="R44" s="7" t="s">
         <v>573</v>
       </c>
-      <c r="S44" t="s">
+      <c r="S44" s="7" t="s">
         <v>574</v>
       </c>
-      <c r="T44" t="s">
+      <c r="T44" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="U44" t="s">
+      <c r="U44" s="7" t="s">
         <v>576</v>
       </c>
-      <c r="V44" t="s">
+      <c r="V44" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W44" t="s">
+      <c r="W44" s="7" t="s">
         <v>577</v>
       </c>
-      <c r="Z44" t="s">
+      <c r="Z44" s="7" t="s">
         <v>578</v>
       </c>
     </row>
@@ -6198,429 +6195,429 @@
         <v>595</v>
       </c>
     </row>
-    <row r="46" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+    <row r="46" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>597</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="10" t="s">
         <v>598</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>599</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="10">
         <v>3.7</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="10">
         <v>70</v>
       </c>
-      <c r="F46" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G46" t="s">
-        <v>1</v>
-      </c>
-      <c r="H46" s="9" t="s">
+      <c r="F46" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" s="10" t="s">
         <v>600</v>
       </c>
-      <c r="I46" s="9" t="s">
+      <c r="I46" s="10" t="s">
         <v>601</v>
       </c>
-      <c r="J46" s="9" t="s">
+      <c r="J46" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K46" s="9" t="s">
+      <c r="K46" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="L46" t="s">
-        <v>1</v>
-      </c>
-      <c r="M46" s="9" t="s">
+      <c r="L46" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M46" s="10" t="s">
         <v>602</v>
       </c>
-      <c r="N46" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="O46" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="P46" s="9" t="s">
+      <c r="N46" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O46" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P46" s="10" t="s">
         <v>603</v>
       </c>
-      <c r="Q46" s="9" t="s">
+      <c r="Q46" s="10" t="s">
         <v>604</v>
       </c>
-      <c r="R46" s="9" t="s">
+      <c r="R46" s="10" t="s">
         <v>605</v>
       </c>
-      <c r="S46" s="9" t="s">
+      <c r="S46" s="10" t="s">
         <v>606</v>
       </c>
-      <c r="T46" s="9" t="s">
+      <c r="T46" s="10" t="s">
         <v>607</v>
       </c>
-      <c r="U46" s="9" t="s">
+      <c r="U46" s="10" t="s">
         <v>608</v>
       </c>
-      <c r="V46" s="9" t="s">
+      <c r="V46" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="W46" s="9" t="s">
+      <c r="W46" s="10" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="47" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>610</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="10" t="s">
         <v>611</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="10" t="s">
         <v>612</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="10">
         <v>5</v>
       </c>
-      <c r="E47" s="9">
-        <v>1</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G47" t="s">
-        <v>1</v>
-      </c>
-      <c r="H47" s="9" t="s">
+      <c r="E47" s="10">
+        <v>1</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" s="10" t="s">
         <v>613</v>
       </c>
-      <c r="I47" s="9" t="s">
+      <c r="I47" s="10" t="s">
         <v>614</v>
       </c>
-      <c r="J47" s="9" t="s">
+      <c r="J47" s="10" t="s">
         <v>615</v>
       </c>
-      <c r="K47" s="9" t="s">
+      <c r="K47" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="L47" t="s">
-        <v>1</v>
-      </c>
-      <c r="M47" s="9" t="s">
+      <c r="L47" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M47" s="10" t="s">
         <v>616</v>
       </c>
-      <c r="N47" s="9" t="s">
+      <c r="N47" s="10" t="s">
         <v>617</v>
       </c>
-      <c r="O47" s="9" t="s">
+      <c r="O47" s="10" t="s">
         <v>617</v>
       </c>
-      <c r="P47" s="9" t="s">
+      <c r="P47" s="10" t="s">
         <v>618</v>
       </c>
-      <c r="Q47" s="9" t="s">
+      <c r="Q47" s="10" t="s">
         <v>619</v>
       </c>
-      <c r="R47" s="9" t="s">
+      <c r="R47" s="10" t="s">
         <v>620</v>
       </c>
-      <c r="S47" s="9" t="s">
+      <c r="S47" s="10" t="s">
         <v>621</v>
       </c>
-      <c r="T47" s="9" t="s">
+      <c r="T47" s="10" t="s">
         <v>622</v>
       </c>
-      <c r="U47" s="9" t="s">
+      <c r="U47" s="10" t="s">
         <v>623</v>
       </c>
-      <c r="V47" s="9" t="s">
+      <c r="V47" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="W47" s="9" t="s">
+      <c r="W47" s="10" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="48" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+    <row r="48" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="10" t="s">
         <v>626</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="10" t="s">
         <v>627</v>
       </c>
-      <c r="D48" s="9">
-        <v>0</v>
-      </c>
-      <c r="E48" s="9">
-        <v>0</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G48" t="s">
-        <v>1</v>
-      </c>
-      <c r="H48" s="9" t="s">
+      <c r="D48" s="10">
+        <v>0</v>
+      </c>
+      <c r="E48" s="10">
+        <v>0</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H48" s="10" t="s">
         <v>628</v>
       </c>
-      <c r="I48" s="9" t="s">
+      <c r="I48" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="J48" s="9" t="s">
+      <c r="J48" s="10" t="s">
         <v>630</v>
       </c>
-      <c r="K48" s="9" t="s">
+      <c r="K48" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="L48" t="s">
-        <v>1</v>
-      </c>
-      <c r="M48" s="9" t="s">
+      <c r="L48" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M48" s="10" t="s">
         <v>631</v>
       </c>
-      <c r="N48" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="O48" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="P48" s="9" t="s">
+      <c r="N48" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P48" s="10" t="s">
         <v>632</v>
       </c>
-      <c r="Q48" s="9" t="s">
+      <c r="Q48" s="10" t="s">
         <v>633</v>
       </c>
-      <c r="R48" s="9" t="s">
+      <c r="R48" s="10" t="s">
         <v>634</v>
       </c>
-      <c r="S48" s="9" t="s">
+      <c r="S48" s="10" t="s">
         <v>635</v>
       </c>
-      <c r="T48" s="9" t="s">
+      <c r="T48" s="10" t="s">
         <v>636</v>
       </c>
-      <c r="U48" s="9" t="s">
+      <c r="U48" s="10" t="s">
         <v>637</v>
       </c>
-      <c r="V48" s="9" t="s">
+      <c r="V48" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="W48" s="9" t="s">
+      <c r="W48" s="10" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="49" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+    <row r="49" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>639</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="10" t="s">
         <v>640</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="10" t="s">
         <v>641</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="10">
         <v>3.8</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="10">
         <v>2</v>
       </c>
-      <c r="F49" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G49" t="s">
-        <v>1</v>
-      </c>
-      <c r="H49" s="9" t="s">
+      <c r="F49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H49" s="10" t="s">
         <v>642</v>
       </c>
-      <c r="I49" s="9" t="s">
+      <c r="I49" s="10" t="s">
         <v>643</v>
       </c>
-      <c r="J49" s="9" t="s">
+      <c r="J49" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="K49" s="9" t="s">
+      <c r="K49" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="L49" t="s">
-        <v>1</v>
-      </c>
-      <c r="M49" s="9" t="s">
+      <c r="L49" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M49" s="10" t="s">
         <v>644</v>
       </c>
-      <c r="N49" s="9" t="s">
+      <c r="N49" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="O49" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="P49" s="9" t="s">
+      <c r="O49" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P49" s="10" t="s">
         <v>645</v>
       </c>
-      <c r="Q49" s="9" t="s">
+      <c r="Q49" s="10" t="s">
         <v>646</v>
       </c>
-      <c r="R49" s="9" t="s">
+      <c r="R49" s="10" t="s">
         <v>647</v>
       </c>
-      <c r="S49" s="9" t="s">
+      <c r="S49" s="10" t="s">
         <v>648</v>
       </c>
-      <c r="T49" s="9" t="s">
+      <c r="T49" s="10" t="s">
         <v>649</v>
       </c>
-      <c r="U49" s="9" t="s">
+      <c r="U49" s="10" t="s">
         <v>650</v>
       </c>
-      <c r="V49" s="9" t="s">
+      <c r="V49" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="W49" s="9" t="s">
+      <c r="W49" s="10" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="50" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+    <row r="50" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>652</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="10" t="s">
         <v>653</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="10" t="s">
         <v>654</v>
       </c>
-      <c r="D50" s="9">
-        <v>1</v>
-      </c>
-      <c r="E50" s="9">
-        <v>1</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G50" t="s">
-        <v>1</v>
-      </c>
-      <c r="H50" s="9" t="s">
+      <c r="D50" s="10">
+        <v>1</v>
+      </c>
+      <c r="E50" s="10">
+        <v>1</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H50" s="10" t="s">
         <v>655</v>
       </c>
-      <c r="I50" s="9" t="s">
+      <c r="I50" s="10" t="s">
         <v>656</v>
       </c>
-      <c r="J50" s="9" t="s">
+      <c r="J50" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K50" s="9" t="s">
+      <c r="K50" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="L50" t="s">
-        <v>1</v>
-      </c>
-      <c r="M50" s="9" t="s">
+      <c r="L50" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M50" s="10" t="s">
         <v>657</v>
       </c>
-      <c r="N50" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="O50" s="9" t="s">
+      <c r="N50" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O50" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="P50" s="9" t="s">
+      <c r="P50" s="10" t="s">
         <v>658</v>
       </c>
-      <c r="Q50" s="9" t="s">
+      <c r="Q50" s="10" t="s">
         <v>659</v>
       </c>
-      <c r="R50" s="9" t="s">
+      <c r="R50" s="10" t="s">
         <v>660</v>
       </c>
-      <c r="S50" s="9" t="s">
+      <c r="S50" s="10" t="s">
         <v>661</v>
       </c>
-      <c r="T50" s="9" t="s">
+      <c r="T50" s="10" t="s">
         <v>662</v>
       </c>
-      <c r="U50" s="9" t="s">
+      <c r="U50" s="10" t="s">
         <v>663</v>
       </c>
-      <c r="V50" s="9" t="s">
+      <c r="V50" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="W50" s="9" t="s">
+      <c r="W50" s="10" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="51" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+    <row r="51" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>665</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="10" t="s">
         <v>666</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="10" t="s">
         <v>667</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="10">
         <v>5</v>
       </c>
-      <c r="E51" s="9">
-        <v>1</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G51" t="s">
-        <v>1</v>
-      </c>
-      <c r="H51" s="9" t="s">
+      <c r="E51" s="10">
+        <v>1</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H51" s="10" t="s">
         <v>668</v>
       </c>
-      <c r="I51" s="9" t="s">
+      <c r="I51" s="10" t="s">
         <v>669</v>
       </c>
-      <c r="J51" s="9" t="s">
+      <c r="J51" s="10" t="s">
         <v>569</v>
       </c>
-      <c r="K51" s="9" t="s">
+      <c r="K51" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="L51" s="9" t="s">
+      <c r="L51" s="10" t="s">
         <v>670</v>
       </c>
-      <c r="M51" s="9" t="s">
+      <c r="M51" s="10" t="s">
         <v>671</v>
       </c>
-      <c r="N51" s="9" t="s">
+      <c r="N51" s="10" t="s">
         <v>672</v>
       </c>
-      <c r="O51" s="9" t="s">
+      <c r="O51" s="10" t="s">
         <v>673</v>
       </c>
-      <c r="P51" s="9" t="s">
+      <c r="P51" s="10" t="s">
         <v>674</v>
       </c>
-      <c r="Q51" s="9" t="s">
+      <c r="Q51" s="10" t="s">
         <v>675</v>
       </c>
-      <c r="R51" s="9" t="s">
+      <c r="R51" s="10" t="s">
         <v>676</v>
       </c>
-      <c r="S51" s="9" t="s">
+      <c r="S51" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="T51" s="9" t="s">
+      <c r="T51" s="10" t="s">
         <v>678</v>
       </c>
-      <c r="U51" s="9" t="s">
+      <c r="U51" s="10" t="s">
         <v>679</v>
       </c>
-      <c r="V51" s="9" t="s">
+      <c r="V51" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="W51" s="9" t="s">
+      <c r="W51" s="10" t="s">
         <v>680</v>
       </c>
     </row>

</xml_diff>